<commit_message>
added more details in the README
</commit_message>
<xml_diff>
--- a/output/erap_data_final.xlsx
+++ b/output/erap_data_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lamthuyvo/Dropbox/teaching/CUNY/2021-fall/forked-repos/2021-10-erap-analysis/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{E57C7EC6-E5E6-8140-8458-5F50C304873C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{F7DCD18F-2E3A-7341-9E40-77CD1A35CF84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1186,7 +1186,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>